<commit_message>
commit@20210606 + MathJax & Mermaid js script to theme. add markdown notes.
</commit_message>
<xml_diff>
--- a/static/media/个人项目列表.xlsx
+++ b/static/media/个人项目列表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\hugo\site\enzo\static\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FC24FD-AE9E-4C4E-BD83-8B9E5A0DA332}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE0A596-AD36-4F8D-8A17-A66B1E356F33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="480" windowWidth="20475" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="180">
   <si>
     <t>https://github.com/sunduoze/NUEDC.git</t>
   </si>
@@ -675,6 +675,22 @@
   </si>
   <si>
     <t>*picoC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/PaPazhao</t>
+  </si>
+  <si>
+    <t>https://github.com/pansila?tab=repositories</t>
+  </si>
+  <si>
+    <t>https://github.com/liangyongxiang?tab=repositories</t>
+  </si>
+  <si>
+    <t>https://github.com/GorgonMeducer?tab=repositories</t>
+  </si>
+  <si>
+    <t>https://github.com/GorgonMeducer/Generic_MCU_Software_Infrastructure</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -770,6 +786,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -789,7 +873,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CEEACA"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1044,760 +1128,784 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C62"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>107</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B16" t="s">
         <v>106</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>109</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B17" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B18" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B19" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B20" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B21" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B22" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>77</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B23" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>92</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B24" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B25" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>36</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B26" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>156</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B27" t="s">
         <v>154</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>41</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B28" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>43</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B29" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>45</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B30" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>63</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B31" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>112</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B32" t="s">
         <v>114</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>75</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B33" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>94</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>62</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B36" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>69</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B37" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>72</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B38" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>81</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B39" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>84</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B40" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>84</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B41" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>165</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B42" t="s">
         <v>164</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>121</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B43" t="s">
         <v>122</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>65</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B44" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>68</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B45" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>67</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B46" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>66</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B47" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>87</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B48" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>116</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B49" t="s">
         <v>117</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>64</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B50" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>136</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B51" t="s">
         <v>135</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>171</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B52" t="s">
         <v>170</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>139</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B53" t="s">
         <v>138</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>158</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B54" t="s">
         <v>159</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>89</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B55" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>101</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B56" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>126</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B57" t="s">
         <v>124</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>152</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B58" t="s">
         <v>153</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>162</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B59" t="s">
         <v>153</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>129</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B60" t="s">
         <v>128</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>130</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B61" t="s">
         <v>131</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>132</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B62" t="s">
         <v>142</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C62" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>140</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B63" t="s">
         <v>143</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>146</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B64" t="s">
         <v>145</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>149</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B66" t="s">
         <v>150</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>166</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>174</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B68" t="s">
         <v>172</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C68" s="3" t="s">
         <v>173</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{B912F37B-5C71-4CF1-85F7-55D16D13FA33}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{2C2B6223-723C-46FC-A796-B0983974F45E}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{73A04852-B1E8-4B89-BD82-17F8E8005099}"/>
-    <hyperlink ref="C6" r:id="rId4" xr:uid="{70216A05-14FF-41C0-8FE0-5B7CAE5C144C}"/>
-    <hyperlink ref="C7" r:id="rId5" xr:uid="{E5C76F3B-DAB7-49D0-A7CA-E482890A7C1D}"/>
-    <hyperlink ref="C8" r:id="rId6" xr:uid="{F1022732-2A88-4F5E-BD6C-64ABC0786348}"/>
-    <hyperlink ref="C12" r:id="rId7" xr:uid="{4181B595-1D41-41D2-9035-1B46CD8D3269}"/>
-    <hyperlink ref="C13" r:id="rId8" xr:uid="{7787BEFC-BB64-4707-A589-E2FBFFD3F026}"/>
-    <hyperlink ref="C14" r:id="rId9" xr:uid="{7BE32479-F338-437A-B788-A0B1305903F5}"/>
-    <hyperlink ref="C15" r:id="rId10" xr:uid="{1ACB9523-384E-43C7-AF55-23BB68096B15}"/>
-    <hyperlink ref="C16" r:id="rId11" xr:uid="{D6328BD9-BDB2-411B-B291-F139BFF3B260}"/>
-    <hyperlink ref="C22" r:id="rId12" xr:uid="{30C720D9-134A-48B1-910E-75ADFB8B0399}"/>
-    <hyperlink ref="C23" r:id="rId13" xr:uid="{9D57F8C7-D4CD-45D8-83EE-1C2D4208AD6D}"/>
-    <hyperlink ref="C24" r:id="rId14" xr:uid="{56750664-F16B-4528-A656-676293304FAF}"/>
-    <hyperlink ref="C39" r:id="rId15" xr:uid="{AD35451A-0769-4172-BC85-90C6CA9B45FD}"/>
-    <hyperlink ref="C40" r:id="rId16" xr:uid="{CA6F3C45-FDEF-41B9-9B2A-9BB386A91DCC}"/>
-    <hyperlink ref="C41" r:id="rId17" xr:uid="{4DD6E754-49F7-41F5-B913-4BD3ADD76ED3}"/>
-    <hyperlink ref="C38" r:id="rId18" xr:uid="{5A7BB9F1-043E-4E44-BCE8-5F07A7007A3A}"/>
-    <hyperlink ref="C44" r:id="rId19" xr:uid="{22BC75D2-7510-41B0-9C37-508886410170}"/>
-    <hyperlink ref="C25" r:id="rId20" xr:uid="{5CC4500C-C8C4-4A08-A1FE-77B3540F3009}"/>
-    <hyperlink ref="C30" r:id="rId21" xr:uid="{FBA1898A-7976-4063-B79A-A91B35067A1D}"/>
-    <hyperlink ref="C31" r:id="rId22" xr:uid="{F8A9217B-3F6C-4750-BE0C-8205A9A5DEC8}"/>
-    <hyperlink ref="C32" r:id="rId23" xr:uid="{B6CC0DCA-5DC2-4C68-9760-62335F53ABCD}"/>
-    <hyperlink ref="C27" r:id="rId24" xr:uid="{033E9590-AE51-446A-95A1-0A2B500866C0}"/>
-    <hyperlink ref="C17" r:id="rId25" xr:uid="{1010FFDD-F69F-4C22-9F8D-968F7BD09CD8}"/>
-    <hyperlink ref="C33" r:id="rId26" xr:uid="{86620C3D-485D-4537-8C96-164E4710E53D}"/>
-    <hyperlink ref="C34" r:id="rId27" xr:uid="{338F331F-AA6A-44A8-B686-2510DC8CEA4E}"/>
-    <hyperlink ref="C42" r:id="rId28" xr:uid="{69F4D2FD-2E13-45F4-8F61-07C765A697B3}"/>
-    <hyperlink ref="C49" r:id="rId29" xr:uid="{FDAB5C3C-8E25-4B37-B640-39E92A1F4A64}"/>
-    <hyperlink ref="C18" r:id="rId30" xr:uid="{D6E892E6-45B8-4551-AE4B-ABDA1CAD8FDC}"/>
-    <hyperlink ref="C28" r:id="rId31" xr:uid="{30EF42AC-AB55-443C-A54C-223433746450}"/>
-    <hyperlink ref="C29" r:id="rId32" xr:uid="{DA2A9B90-AA8D-4CED-B396-3F8CCAEAC290}"/>
-    <hyperlink ref="C19" r:id="rId33" xr:uid="{F7BE3E00-732F-4373-A731-A37B5DC199C2}"/>
-    <hyperlink ref="C50" r:id="rId34" xr:uid="{D6594FCA-981B-4216-8425-4FDA36F71900}"/>
-    <hyperlink ref="C9" r:id="rId35" xr:uid="{9FE3BB6F-7E18-4D57-9D8B-77794A752904}"/>
-    <hyperlink ref="C10" r:id="rId36" xr:uid="{6A6E113D-87C4-45B2-95AD-6DBBD56D5E08}"/>
-    <hyperlink ref="C11" r:id="rId37" xr:uid="{6E7BF21A-B042-4345-9846-1B221F5CDC5A}"/>
-    <hyperlink ref="C26" r:id="rId38" xr:uid="{4C055CF9-5435-4C10-85E3-536634BE22F5}"/>
-    <hyperlink ref="C43" r:id="rId39" xr:uid="{B0C9FF40-A05B-4035-BAF2-BAE5AE81D669}"/>
-    <hyperlink ref="C20" r:id="rId40" xr:uid="{346B9181-876E-4F7D-8A21-19526C8CB281}"/>
-    <hyperlink ref="C37" r:id="rId41" xr:uid="{444C4505-7E57-4899-9608-80888183B5FC}"/>
-    <hyperlink ref="C51" r:id="rId42" xr:uid="{A1BCE9A4-8D74-409A-8DC1-B13A39259031}"/>
-    <hyperlink ref="B51" r:id="rId43" display="https://github.com/sunduoze/stm32flash" xr:uid="{4FC6FAC7-A7E7-4E32-940C-109F2ADC761C}"/>
-    <hyperlink ref="C55" r:id="rId44" xr:uid="{428FFAF5-9DF8-4D2B-8434-D746395852F1}"/>
-    <hyperlink ref="C54" r:id="rId45" xr:uid="{7B63DBA4-B02E-4D4A-84D8-49FE07AE104B}"/>
-    <hyperlink ref="C56" r:id="rId46" xr:uid="{4675D027-734D-49C6-A42F-52F99DBF7524}"/>
-    <hyperlink ref="C45" r:id="rId47" xr:uid="{C2304F45-EADE-40C9-9C00-4B3C141DA3FC}"/>
-    <hyperlink ref="C47" r:id="rId48" xr:uid="{062E1526-AEAA-42D7-9256-88B229F6229D}"/>
-    <hyperlink ref="C57" r:id="rId49" xr:uid="{54B5F288-1036-4EB7-8630-41174C843BF7}"/>
-    <hyperlink ref="C58" r:id="rId50" xr:uid="{B63E9D6B-4AB9-4621-933E-265FAC8FD9C0}"/>
-    <hyperlink ref="C60" r:id="rId51" xr:uid="{5E9511C2-477F-4B96-96D1-6C3F01FA9C86}"/>
-    <hyperlink ref="C52" r:id="rId52" xr:uid="{33B05090-31B7-473F-8FE2-AB6121F432FB}"/>
-    <hyperlink ref="C21" r:id="rId53" xr:uid="{7191D2F4-2C87-46E9-8D40-87195AE2B9AD}"/>
-    <hyperlink ref="C48" r:id="rId54" xr:uid="{D786CFB5-A3A7-4CFC-8D2C-8DA1DF529003}"/>
-    <hyperlink ref="C35" r:id="rId55" xr:uid="{EE5A8341-A21D-47A5-9EE9-316E7074D807}"/>
-    <hyperlink ref="C53" r:id="rId56" xr:uid="{E970C138-F013-4E5F-A21D-B1FD9D0C0931}"/>
-    <hyperlink ref="C36" r:id="rId57" xr:uid="{EE1DACDE-303E-43E1-AC24-AE4BE9CFD483}"/>
-    <hyperlink ref="C61" r:id="rId58" xr:uid="{7220AC08-CA2B-42C7-8216-FE9961188C77}"/>
-    <hyperlink ref="C46" r:id="rId59" xr:uid="{DF68B1A5-3714-45BD-B9D3-4D403D2184C4}"/>
-    <hyperlink ref="C62" r:id="rId60" xr:uid="{A9963403-E4A9-4CEA-90D6-BDDCD6151953}"/>
+    <hyperlink ref="C9" r:id="rId1" xr:uid="{B912F37B-5C71-4CF1-85F7-55D16D13FA33}"/>
+    <hyperlink ref="C10" r:id="rId2" xr:uid="{2C2B6223-723C-46FC-A796-B0983974F45E}"/>
+    <hyperlink ref="C11" r:id="rId3" xr:uid="{73A04852-B1E8-4B89-BD82-17F8E8005099}"/>
+    <hyperlink ref="C12" r:id="rId4" xr:uid="{70216A05-14FF-41C0-8FE0-5B7CAE5C144C}"/>
+    <hyperlink ref="C13" r:id="rId5" xr:uid="{E5C76F3B-DAB7-49D0-A7CA-E482890A7C1D}"/>
+    <hyperlink ref="C14" r:id="rId6" xr:uid="{F1022732-2A88-4F5E-BD6C-64ABC0786348}"/>
+    <hyperlink ref="C18" r:id="rId7" xr:uid="{4181B595-1D41-41D2-9035-1B46CD8D3269}"/>
+    <hyperlink ref="C19" r:id="rId8" xr:uid="{7787BEFC-BB64-4707-A589-E2FBFFD3F026}"/>
+    <hyperlink ref="C20" r:id="rId9" xr:uid="{7BE32479-F338-437A-B788-A0B1305903F5}"/>
+    <hyperlink ref="C21" r:id="rId10" xr:uid="{1ACB9523-384E-43C7-AF55-23BB68096B15}"/>
+    <hyperlink ref="C22" r:id="rId11" xr:uid="{D6328BD9-BDB2-411B-B291-F139BFF3B260}"/>
+    <hyperlink ref="C28" r:id="rId12" xr:uid="{30C720D9-134A-48B1-910E-75ADFB8B0399}"/>
+    <hyperlink ref="C29" r:id="rId13" xr:uid="{9D57F8C7-D4CD-45D8-83EE-1C2D4208AD6D}"/>
+    <hyperlink ref="C30" r:id="rId14" xr:uid="{56750664-F16B-4528-A656-676293304FAF}"/>
+    <hyperlink ref="C45" r:id="rId15" xr:uid="{AD35451A-0769-4172-BC85-90C6CA9B45FD}"/>
+    <hyperlink ref="C46" r:id="rId16" xr:uid="{CA6F3C45-FDEF-41B9-9B2A-9BB386A91DCC}"/>
+    <hyperlink ref="C47" r:id="rId17" xr:uid="{4DD6E754-49F7-41F5-B913-4BD3ADD76ED3}"/>
+    <hyperlink ref="C44" r:id="rId18" xr:uid="{5A7BB9F1-043E-4E44-BCE8-5F07A7007A3A}"/>
+    <hyperlink ref="C50" r:id="rId19" xr:uid="{22BC75D2-7510-41B0-9C37-508886410170}"/>
+    <hyperlink ref="C31" r:id="rId20" xr:uid="{5CC4500C-C8C4-4A08-A1FE-77B3540F3009}"/>
+    <hyperlink ref="C36" r:id="rId21" xr:uid="{FBA1898A-7976-4063-B79A-A91B35067A1D}"/>
+    <hyperlink ref="C37" r:id="rId22" xr:uid="{F8A9217B-3F6C-4750-BE0C-8205A9A5DEC8}"/>
+    <hyperlink ref="C38" r:id="rId23" xr:uid="{B6CC0DCA-5DC2-4C68-9760-62335F53ABCD}"/>
+    <hyperlink ref="C33" r:id="rId24" xr:uid="{033E9590-AE51-446A-95A1-0A2B500866C0}"/>
+    <hyperlink ref="C23" r:id="rId25" xr:uid="{1010FFDD-F69F-4C22-9F8D-968F7BD09CD8}"/>
+    <hyperlink ref="C39" r:id="rId26" xr:uid="{86620C3D-485D-4537-8C96-164E4710E53D}"/>
+    <hyperlink ref="C40" r:id="rId27" xr:uid="{338F331F-AA6A-44A8-B686-2510DC8CEA4E}"/>
+    <hyperlink ref="C48" r:id="rId28" xr:uid="{69F4D2FD-2E13-45F4-8F61-07C765A697B3}"/>
+    <hyperlink ref="C55" r:id="rId29" xr:uid="{FDAB5C3C-8E25-4B37-B640-39E92A1F4A64}"/>
+    <hyperlink ref="C24" r:id="rId30" xr:uid="{D6E892E6-45B8-4551-AE4B-ABDA1CAD8FDC}"/>
+    <hyperlink ref="C34" r:id="rId31" xr:uid="{30EF42AC-AB55-443C-A54C-223433746450}"/>
+    <hyperlink ref="C35" r:id="rId32" xr:uid="{DA2A9B90-AA8D-4CED-B396-3F8CCAEAC290}"/>
+    <hyperlink ref="C25" r:id="rId33" xr:uid="{F7BE3E00-732F-4373-A731-A37B5DC199C2}"/>
+    <hyperlink ref="C56" r:id="rId34" xr:uid="{D6594FCA-981B-4216-8425-4FDA36F71900}"/>
+    <hyperlink ref="C15" r:id="rId35" xr:uid="{9FE3BB6F-7E18-4D57-9D8B-77794A752904}"/>
+    <hyperlink ref="C16" r:id="rId36" xr:uid="{6A6E113D-87C4-45B2-95AD-6DBBD56D5E08}"/>
+    <hyperlink ref="C17" r:id="rId37" xr:uid="{6E7BF21A-B042-4345-9846-1B221F5CDC5A}"/>
+    <hyperlink ref="C32" r:id="rId38" xr:uid="{4C055CF9-5435-4C10-85E3-536634BE22F5}"/>
+    <hyperlink ref="C49" r:id="rId39" xr:uid="{B0C9FF40-A05B-4035-BAF2-BAE5AE81D669}"/>
+    <hyperlink ref="C26" r:id="rId40" xr:uid="{346B9181-876E-4F7D-8A21-19526C8CB281}"/>
+    <hyperlink ref="C43" r:id="rId41" xr:uid="{444C4505-7E57-4899-9608-80888183B5FC}"/>
+    <hyperlink ref="C57" r:id="rId42" xr:uid="{A1BCE9A4-8D74-409A-8DC1-B13A39259031}"/>
+    <hyperlink ref="B57" r:id="rId43" display="https://github.com/sunduoze/stm32flash" xr:uid="{4FC6FAC7-A7E7-4E32-940C-109F2ADC761C}"/>
+    <hyperlink ref="C61" r:id="rId44" xr:uid="{428FFAF5-9DF8-4D2B-8434-D746395852F1}"/>
+    <hyperlink ref="C60" r:id="rId45" xr:uid="{7B63DBA4-B02E-4D4A-84D8-49FE07AE104B}"/>
+    <hyperlink ref="C62" r:id="rId46" xr:uid="{4675D027-734D-49C6-A42F-52F99DBF7524}"/>
+    <hyperlink ref="C51" r:id="rId47" xr:uid="{C2304F45-EADE-40C9-9C00-4B3C141DA3FC}"/>
+    <hyperlink ref="C53" r:id="rId48" xr:uid="{062E1526-AEAA-42D7-9256-88B229F6229D}"/>
+    <hyperlink ref="C63" r:id="rId49" xr:uid="{54B5F288-1036-4EB7-8630-41174C843BF7}"/>
+    <hyperlink ref="C64" r:id="rId50" xr:uid="{B63E9D6B-4AB9-4621-933E-265FAC8FD9C0}"/>
+    <hyperlink ref="C66" r:id="rId51" xr:uid="{5E9511C2-477F-4B96-96D1-6C3F01FA9C86}"/>
+    <hyperlink ref="C58" r:id="rId52" xr:uid="{33B05090-31B7-473F-8FE2-AB6121F432FB}"/>
+    <hyperlink ref="C27" r:id="rId53" xr:uid="{7191D2F4-2C87-46E9-8D40-87195AE2B9AD}"/>
+    <hyperlink ref="C54" r:id="rId54" xr:uid="{D786CFB5-A3A7-4CFC-8D2C-8DA1DF529003}"/>
+    <hyperlink ref="C41" r:id="rId55" xr:uid="{EE5A8341-A21D-47A5-9EE9-316E7074D807}"/>
+    <hyperlink ref="C59" r:id="rId56" xr:uid="{E970C138-F013-4E5F-A21D-B1FD9D0C0931}"/>
+    <hyperlink ref="C42" r:id="rId57" xr:uid="{EE1DACDE-303E-43E1-AC24-AE4BE9CFD483}"/>
+    <hyperlink ref="C67" r:id="rId58" xr:uid="{7220AC08-CA2B-42C7-8216-FE9961188C77}"/>
+    <hyperlink ref="C52" r:id="rId59" xr:uid="{DF68B1A5-3714-45BD-B9D3-4D403D2184C4}"/>
+    <hyperlink ref="C68" r:id="rId60" xr:uid="{A9963403-E4A9-4CEA-90D6-BDDCD6151953}"/>
+    <hyperlink ref="C1" r:id="rId61" xr:uid="{E470E0AB-AAE7-41D8-83C0-E1C9B55D67B5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId61"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId62"/>
 </worksheet>
 </file>
</xml_diff>